<commit_message>
Final and with docker version
</commit_message>
<xml_diff>
--- a/assets/template_siswa.xlsx
+++ b/assets/template_siswa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\apdate_v2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2973F421-3F10-44C0-A608-E37C22378503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645FD8AD-DF4A-4382-89D9-FB162B82BAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0DBB2CD0-9512-4F4E-A4E1-BC74892CCADA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Muhammad Ichsan Fathurrochman</t>
   </si>
@@ -157,13 +157,28 @@
   </si>
   <si>
     <t>Seniman</t>
+  </si>
+  <si>
+    <t>Budi Ahmad Jaya</t>
+  </si>
+  <si>
+    <t>budi.aj@email.com</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>Indah</t>
+  </si>
+  <si>
+    <t>siswa_baru_tingkat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +192,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -209,11 +232,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -231,8 +266,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9067D0B-209A-42C7-8D94-AA7FFDBD9207}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,9 +606,15 @@
     <col min="13" max="13" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -616,8 +660,29 @@
       <c r="O1" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="P1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1220014</v>
       </c>
@@ -663,8 +728,29 @@
       <c r="O2" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="P2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="5">
+        <v>87788990011</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1220015</v>
       </c>
@@ -693,25 +779,46 @@
         <v>28</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="K3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3" s="5">
+        <v>81122334455</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="5">
+      <c r="S3" s="5">
         <v>87788990011</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="T3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="V3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1220016</v>
       </c>
@@ -757,8 +864,32 @@
       <c r="O4" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="P4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="5">
+        <v>87788990011</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="V4">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N3" r:id="rId1" xr:uid="{D9E675C6-1EFC-471A-AE1F-07059B2A96CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>